<commit_message>
feat(elec): add 'source' info to provision certificates
</commit_message>
<xml_diff>
--- a/front/public/templates/certificats-de-fourniture.xlsx
+++ b/front/public/templates/certificats-de-fourniture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yohann/Documents/Projets/YomiCode/CarbuRe/carbure/front/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D69E66-3412-0140-A64D-30367C660AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39028F8-51D6-D04E-B106-430D855EE76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>cpo</t>
   </si>
@@ -37,29 +37,20 @@
     <t>energy_amount</t>
   </si>
   <si>
-    <t>current_type</t>
-  </si>
-  <si>
     <t>Aménageur Test</t>
   </si>
   <si>
     <t>FRIONO</t>
   </si>
   <si>
-    <t>CC</t>
-  </si>
-  <si>
     <t>AZERTO</t>
-  </si>
-  <si>
-    <t>AC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -77,21 +68,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -115,12 +91,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,19 +313,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X20"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -367,9 +342,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -387,11 +360,10 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-    </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -400,18 +372,15 @@
         <v>2022</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2">
         <v>20000</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -420,100 +389,97 @@
         <v>2023</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
         <v>2000</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>